<commit_message>
Modified player insert to avoid a NOT NULL violation trying to insert a NULL `create_date` instead of NOW().
</commit_message>
<xml_diff>
--- a/cardshifter-database/cardshifter-0.4-player-list.xlsx
+++ b/cardshifter-database/cardshifter-0.4-player-list.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="10">
   <si>
     <t>id</t>
   </si>
@@ -55,7 +55,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -68,13 +68,35 @@
       <color theme="1"/>
       <name val="Consolas"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -86,14 +108,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,14 +472,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.83203125" style="1"/>
   </cols>
@@ -468,7 +514,7 @@
       <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H3" t="s">
@@ -478,8 +524,8 @@
         <v>8</v>
       </c>
       <c r="J3" s="1" t="str">
-        <f>"INSERT INTO player("&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;","&amp;I3&amp;") VALUES"</f>
-        <v>INSERT INTO player(name,password,email,website,about,create_date,delete_date,last_seen_date) VALUES</v>
+        <f>"INSERT INTO player("&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;H3&amp;","&amp;I3&amp;") VALUES"</f>
+        <v>INSERT INTO player(name,password,email,website,about,delete_date,last_seen_date) VALUES</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -500,9 +546,6 @@
       <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
       <c r="H4" t="s">
         <v>9</v>
       </c>
@@ -510,8 +553,8 @@
         <v>9</v>
       </c>
       <c r="J4" s="1" t="str">
-        <f>"("&amp;B4&amp;","&amp;C4&amp;","&amp;D4&amp;","&amp;E4&amp;","&amp;F4&amp;","&amp;G4&amp;","&amp;H4&amp;","&amp;I4&amp;"),"</f>
-        <v>('Zomis','*****',null,null,null,null,null,null),</v>
+        <f>"("&amp;B4&amp;","&amp;C4&amp;","&amp;D4&amp;","&amp;E4&amp;","&amp;F4&amp;","&amp;H4&amp;","&amp;I4&amp;"),"</f>
+        <v>('Zomis','*****',null,null,null,null,null),</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -532,9 +575,6 @@
       <c r="F5" t="s">
         <v>9</v>
       </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
       <c r="H5" t="s">
         <v>9</v>
       </c>
@@ -542,8 +582,8 @@
         <v>9</v>
       </c>
       <c r="J5" s="1" t="str">
-        <f t="shared" ref="J5:J9" si="1">"("&amp;B5&amp;","&amp;C5&amp;","&amp;D5&amp;","&amp;E5&amp;","&amp;F5&amp;","&amp;G5&amp;","&amp;H5&amp;","&amp;I5&amp;"),"</f>
-        <v>('bazola','*****',null,null,null,null,null,null),</v>
+        <f t="shared" ref="J5:J10" si="1">"("&amp;B5&amp;","&amp;C5&amp;","&amp;D5&amp;","&amp;E5&amp;","&amp;F5&amp;","&amp;H5&amp;","&amp;I5&amp;"),"</f>
+        <v>('bazola','*****',null,null,null,null,null),</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -564,9 +604,6 @@
       <c r="F6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
       <c r="H6" t="s">
         <v>9</v>
       </c>
@@ -575,7 +612,7 @@
       </c>
       <c r="J6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>('skiwi','*****',null,null,null,null,null,null),</v>
+        <v>('skiwi','*****',null,null,null,null,null),</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -596,9 +633,6 @@
       <c r="F7" t="s">
         <v>9</v>
       </c>
-      <c r="G7" t="s">
-        <v>9</v>
-      </c>
       <c r="H7" t="s">
         <v>9</v>
       </c>
@@ -607,7 +641,7 @@
       </c>
       <c r="J7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>('Phrancis','*****',null,null,null,null,null,null),</v>
+        <v>('Phrancis','*****',null,null,null,null,null),</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -628,9 +662,6 @@
       <c r="F8" t="s">
         <v>9</v>
       </c>
-      <c r="G8" t="s">
-        <v>9</v>
-      </c>
       <c r="H8" t="s">
         <v>9</v>
       </c>
@@ -639,7 +670,7 @@
       </c>
       <c r="J8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>('GreyFox','*****',null,null,null,null,null,null),</v>
+        <v>('GreyFox','*****',null,null,null,null,null),</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -660,9 +691,6 @@
       <c r="F9" t="s">
         <v>9</v>
       </c>
-      <c r="G9" t="s">
-        <v>9</v>
-      </c>
       <c r="H9" t="s">
         <v>9</v>
       </c>
@@ -670,8 +698,8 @@
         <v>9</v>
       </c>
       <c r="J9" s="1" t="str">
-        <f>"("&amp;B9&amp;","&amp;C9&amp;","&amp;D9&amp;","&amp;E9&amp;","&amp;F9&amp;","&amp;G9&amp;","&amp;H9&amp;","&amp;I9&amp;");"</f>
-        <v>('Jay1148','*****',null,null,null,null,null,null);</v>
+        <f>"("&amp;B9&amp;","&amp;C9&amp;","&amp;D9&amp;","&amp;E9&amp;","&amp;F9&amp;","&amp;H9&amp;","&amp;I9&amp;");"</f>
+        <v>('Jay1148','*****',null,null,null,null,null);</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -682,6 +710,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>